<commit_message>
Updated Samples.xlsx and added QID/References
</commit_message>
<xml_diff>
--- a/Microplastic_Data_Portal-main/data/Microplastics_DataPortal_Clean_Morphology.xlsx
+++ b/Microplastic_Data_Portal-main/data/Microplastics_DataPortal_Clean_Morphology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastics in Drinking Water/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastic_Data_Portal-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6599FF7-8C27-5545-A931-A82EC0B278AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EAE275-20E2-4F4F-9859-9705428FA597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="500" windowWidth="10000" windowHeight="16940" xr2:uid="{D401F74E-A2D1-9C4E-9D2D-23BF4F6F8055}"/>
+    <workbookView xWindow="10020" yWindow="500" windowWidth="10920" windowHeight="11880" xr2:uid="{D401F74E-A2D1-9C4E-9D2D-23BF4F6F8055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Morphology</t>
   </si>
@@ -104,16 +104,86 @@
   </si>
   <si>
     <t>Sheets</t>
+  </si>
+  <si>
+    <t>Locked (Y/N)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Primary Alias</t>
+  </si>
+  <si>
+    <t>Thin Film</t>
+  </si>
+  <si>
+    <t>Nurdle</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>QID</t>
+  </si>
+  <si>
+    <t>Q66539740</t>
+  </si>
+  <si>
+    <t>Q11086567</t>
+  </si>
+  <si>
+    <t>Q161</t>
+  </si>
+  <si>
+    <t>Q109875324</t>
+  </si>
+  <si>
+    <t>Q1137203</t>
+  </si>
+  <si>
+    <t>Q215414</t>
+  </si>
+  <si>
+    <t>Q12507</t>
+  </si>
+  <si>
+    <t>Q37105</t>
+  </si>
+  <si>
+    <t>Q1053956</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>10.3389/fchem.2018.00407</t>
+  </si>
+  <si>
+    <t>10.1016/j.watres.2019.02.054</t>
+  </si>
+  <si>
+    <t>10.1007/s11783-021-1492-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,105 +526,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31FD0F3-3196-1440-93E1-E0A09F303C3A}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>